<commit_message>
fixed null values and added sorting
</commit_message>
<xml_diff>
--- a/src/main/resources/routes/dev-data.xlsx
+++ b/src/main/resources/routes/dev-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\IdeaProjects\locationSender\src\main\resources\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACBD104-72FB-424F-AA06-8AAB6025EB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AA77A9-FED8-4A74-9E3B-BC5646165BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dev1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +530,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="3">
-        <v>133982</v>
+        <v>13434</v>
       </c>
       <c r="F3" s="3">
         <v>5</v>
@@ -562,7 +562,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="3">
-        <v>267813</v>
+        <v>14343</v>
       </c>
       <c r="F4" s="3">
         <v>6</v>
@@ -594,7 +594,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="3">
-        <v>401928</v>
+        <v>15342</v>
       </c>
       <c r="F5" s="3">
         <v>6</v>
@@ -626,7 +626,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="3">
-        <v>530032</v>
+        <v>16342</v>
       </c>
       <c r="F6" s="3">
         <v>7</v>
@@ -658,7 +658,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="3">
-        <v>668321</v>
+        <v>17121</v>
       </c>
       <c r="F7" s="3">
         <v>7</v>
@@ -690,7 +690,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="3">
-        <v>798127</v>
+        <v>17900</v>
       </c>
       <c r="F8" s="3">
         <v>7</v>
@@ -722,7 +722,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="3">
-        <v>9832</v>
+        <v>18123</v>
       </c>
       <c r="F9" s="3">
         <v>5</v>
@@ -754,7 +754,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="3">
-        <v>98291</v>
+        <v>19234</v>
       </c>
       <c r="F10" s="3">
         <v>5</v>
@@ -786,7 +786,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="3">
-        <v>183273</v>
+        <v>20123</v>
       </c>
       <c r="F11" s="3">
         <v>5</v>
@@ -818,7 +818,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="3">
-        <v>278127</v>
+        <v>22234</v>
       </c>
       <c r="F12" s="3">
         <v>6</v>
@@ -850,7 +850,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="3">
-        <v>372819</v>
+        <v>23123</v>
       </c>
       <c r="F13" s="3">
         <v>6</v>
@@ -882,7 +882,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="3">
-        <v>469912</v>
+        <v>23999</v>
       </c>
       <c r="F14" s="3">
         <v>6</v>
@@ -914,7 +914,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="3">
-        <v>545913</v>
+        <v>24990</v>
       </c>
       <c r="F15" s="3">
         <v>7</v>
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="3">
-        <v>645456</v>
+        <v>26000</v>
       </c>
       <c r="F16" s="3">
         <v>8</v>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A50759-DB11-47C5-ADD2-AEDB042843BE}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,7 +1025,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="3">
-        <v>93429</v>
+        <v>1231</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -1057,7 +1057,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="3">
-        <v>202575</v>
+        <v>4231</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
@@ -1089,7 +1089,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="3">
-        <v>284259</v>
+        <v>5231</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
@@ -1121,7 +1121,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>736935</v>
+        <v>7231</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
@@ -1153,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="3">
-        <v>1211279</v>
+        <v>8123</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>13</v>
@@ -1181,7 +1181,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1338,9 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C195135-D785-4179-B46D-6DEDE81761E4}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1417,7 +1415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8E02C7-3180-49A8-8DAF-9BB4809F256B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1785,7 +1783,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1868,7 +1866,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="3">
-        <v>60837</v>
+        <v>33000</v>
       </c>
       <c r="F3" s="3">
         <v>3</v>
@@ -1900,7 +1898,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="3">
-        <v>91456</v>
+        <v>34000</v>
       </c>
       <c r="F4" s="3">
         <v>3</v>
@@ -1932,7 +1930,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="3">
-        <v>130981</v>
+        <v>35121</v>
       </c>
       <c r="F5" s="3">
         <v>3</v>
@@ -1964,7 +1962,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="3">
-        <v>160873</v>
+        <v>36123</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
@@ -1996,7 +1994,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="3">
-        <v>193475</v>
+        <v>36812</v>
       </c>
       <c r="F7" s="3">
         <v>3</v>
@@ -2028,7 +2026,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="3">
-        <v>217847</v>
+        <v>39123</v>
       </c>
       <c r="F8" s="3">
         <v>3</v>
@@ -2060,7 +2058,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="3">
-        <v>246891</v>
+        <v>40000</v>
       </c>
       <c r="F9" s="3">
         <v>3</v>
@@ -2092,7 +2090,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="3">
-        <v>278198</v>
+        <v>41221</v>
       </c>
       <c r="F10" s="3">
         <v>3</v>
@@ -2124,7 +2122,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="3">
-        <v>318233</v>
+        <v>42123</v>
       </c>
       <c r="F11" s="3">
         <v>3</v>
@@ -2152,7 +2150,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2267,7 +2265,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3">
-        <v>12785</v>
+        <v>6234</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
@@ -2299,7 +2297,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="3">
-        <v>17636</v>
+        <v>7533</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
@@ -2331,7 +2329,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="3">
-        <v>23971</v>
+        <v>8123</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>13</v>
@@ -2363,7 +2361,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="3">
-        <v>29769</v>
+        <v>9145</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
@@ -2395,7 +2393,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="3">
-        <v>34521</v>
+        <v>10654</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
@@ -2427,7 +2425,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="3">
-        <v>40818</v>
+        <v>12451</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>13</v>
@@ -2455,7 +2453,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:J16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2538,7 +2536,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="3">
-        <v>133982</v>
+        <v>13213</v>
       </c>
       <c r="F3" s="3">
         <v>5</v>
@@ -2570,7 +2568,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="3">
-        <v>267813</v>
+        <v>14522</v>
       </c>
       <c r="F4" s="3">
         <v>6</v>
@@ -2602,7 +2600,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="3">
-        <v>401928</v>
+        <v>15532</v>
       </c>
       <c r="F5" s="3">
         <v>6</v>
@@ -2634,7 +2632,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="3">
-        <v>530032</v>
+        <v>16093</v>
       </c>
       <c r="F6" s="3">
         <v>7</v>
@@ -2666,7 +2664,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="3">
-        <v>668321</v>
+        <v>17342</v>
       </c>
       <c r="F7" s="3">
         <v>7</v>
@@ -2698,7 +2696,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="3">
-        <v>798127</v>
+        <v>18340</v>
       </c>
       <c r="F8" s="3">
         <v>7</v>
@@ -2762,7 +2760,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="3">
-        <v>98291</v>
+        <v>11234</v>
       </c>
       <c r="F10" s="3">
         <v>5</v>
@@ -2794,7 +2792,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="3">
-        <v>183273</v>
+        <v>13234</v>
       </c>
       <c r="F11" s="3">
         <v>5</v>
@@ -2826,7 +2824,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="3">
-        <v>278127</v>
+        <v>14542</v>
       </c>
       <c r="F12" s="3">
         <v>6</v>
@@ -2858,7 +2856,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="3">
-        <v>372819</v>
+        <v>17934</v>
       </c>
       <c r="F13" s="3">
         <v>6</v>
@@ -2890,7 +2888,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="3">
-        <v>469912</v>
+        <v>19324</v>
       </c>
       <c r="F14" s="3">
         <v>6</v>
@@ -2922,7 +2920,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="3">
-        <v>545913</v>
+        <v>20000</v>
       </c>
       <c r="F15" s="3">
         <v>7</v>
@@ -2954,7 +2952,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="3">
-        <v>645456</v>
+        <v>21453</v>
       </c>
       <c r="F16" s="3">
         <v>8</v>
@@ -2982,7 +2980,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3065,7 +3063,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="4">
-        <v>11401</v>
+        <v>7343</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
@@ -3097,7 +3095,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="4">
-        <v>16587</v>
+        <v>8231</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
@@ -3129,7 +3127,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="4">
-        <v>22478</v>
+        <v>9422</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
@@ -3161,7 +3159,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="4">
-        <v>27731</v>
+        <v>10234</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>13</v>
@@ -3193,7 +3191,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="4">
-        <v>33435</v>
+        <v>12430</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
@@ -3225,7 +3223,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="4">
-        <v>38750</v>
+        <v>13401</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
@@ -3257,7 +3255,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="4">
-        <v>44006</v>
+        <v>14933</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>13</v>
@@ -3289,7 +3287,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="4">
-        <v>49284</v>
+        <v>16123</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>13</v>
@@ -3321,7 +3319,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="4">
-        <v>55117</v>
+        <v>17390</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>13</v>
@@ -3353,7 +3351,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="4">
-        <v>60971</v>
+        <v>18231</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>13</v>
@@ -3385,7 +3383,7 @@
         <v>18</v>
       </c>
       <c r="E13" s="4">
-        <v>66118</v>
+        <v>19234</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>13</v>
@@ -3417,7 +3415,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="4">
-        <v>71481</v>
+        <v>20542</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>13</v>
@@ -3449,7 +3447,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="4">
-        <v>76894</v>
+        <v>22034</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>13</v>
@@ -3481,7 +3479,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="4">
-        <v>82145</v>
+        <v>23400</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>13</v>
@@ -3513,7 +3511,7 @@
         <v>18</v>
       </c>
       <c r="E17" s="4">
-        <v>87595</v>
+        <v>24013</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>13</v>
@@ -3545,7 +3543,7 @@
         <v>18</v>
       </c>
       <c r="E18" s="4">
-        <v>93277</v>
+        <v>27193</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>13</v>
@@ -3577,7 +3575,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="4">
-        <v>98692</v>
+        <v>29012</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>13</v>

</xml_diff>